<commit_message>
Integrated SCiV core with testbech
</commit_message>
<xml_diff>
--- a/doc/isa_dcode.xlsx
+++ b/doc/isa_dcode.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="247">
   <si>
     <t xml:space="preserve">bbr_type</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">src2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC_ADDR</t>
   </si>
   <si>
     <t xml:space="preserve">op_sign</t>
@@ -773,6 +776,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -859,7 +863,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -878,6 +882,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -967,11 +975,11 @@
   </sheetPr>
   <dimension ref="A2:AH54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB7" activeCellId="0" sqref="AB7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P54" activeCellId="0" sqref="P54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -983,12 +991,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="7.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="7.82"/>
@@ -996,11 +1004,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="33.09"/>
   </cols>
   <sheetData>
@@ -1370,12 +1378,14 @@
       <c r="O11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="P11" s="2"/>
+      <c r="P11" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="Q11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>5</v>
@@ -1384,44 +1394,44 @@
         <v>6</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AH11" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1498,46 +1508,49 @@
         <v>0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>37</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="N13" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="P13" s="3" t="str">
+        <f aca="false">DEC2HEX(A13)</f>
+        <v>0</v>
+      </c>
       <c r="Q13" s="2" t="n">
         <v>1</v>
       </c>
@@ -1595,46 +1608,49 @@
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="N14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
+      <c r="P14" s="3" t="str">
+        <f aca="false">DEC2HEX(A14)</f>
+        <v>1</v>
+      </c>
       <c r="Q14" s="2" t="n">
         <v>1</v>
       </c>
@@ -1692,48 +1708,51 @@
         <v>2</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="F15" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="G15" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>34</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="P15" s="3"/>
+        <v>92</v>
+      </c>
+      <c r="P15" s="3" t="str">
+        <f aca="false">DEC2HEX(A15)</f>
+        <v>2</v>
+      </c>
       <c r="Q15" s="2" t="n">
         <v>1</v>
       </c>
@@ -1791,16 +1810,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>67</v>
@@ -1809,19 +1828,19 @@
         <v>0</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>34</v>
@@ -1832,7 +1851,10 @@
       <c r="O16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="3"/>
+      <c r="P16" s="3" t="str">
+        <f aca="false">DEC2HEX(A16)</f>
+        <v>3</v>
+      </c>
       <c r="Q16" s="2" t="n">
         <v>1</v>
       </c>
@@ -1890,16 +1912,16 @@
         <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F17" s="3" t="n">
         <v>63</v>
@@ -1908,22 +1930,22 @@
         <v>0</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>21</v>
@@ -1931,7 +1953,10 @@
       <c r="O17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P17" s="3"/>
+      <c r="P17" s="3" t="str">
+        <f aca="false">DEC2HEX(A17)</f>
+        <v>4</v>
+      </c>
       <c r="Q17" s="2" t="n">
         <v>1</v>
       </c>
@@ -1989,38 +2014,38 @@
         <v>5</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>21</v>
@@ -2028,7 +2053,10 @@
       <c r="O18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P18" s="3"/>
+      <c r="P18" s="3" t="str">
+        <f aca="false">DEC2HEX(A18)</f>
+        <v>5</v>
+      </c>
       <c r="Q18" s="2" t="n">
         <v>1</v>
       </c>
@@ -2086,38 +2114,38 @@
         <v>6</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="n">
         <v>4</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>21</v>
@@ -2125,7 +2153,10 @@
       <c r="O19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P19" s="3"/>
+      <c r="P19" s="3" t="str">
+        <f aca="false">DEC2HEX(A19)</f>
+        <v>6</v>
+      </c>
       <c r="Q19" s="2" t="n">
         <v>1</v>
       </c>
@@ -2183,38 +2214,38 @@
         <v>7</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="n">
         <v>5</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>21</v>
@@ -2222,7 +2253,10 @@
       <c r="O20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P20" s="3"/>
+      <c r="P20" s="3" t="str">
+        <f aca="false">DEC2HEX(A20)</f>
+        <v>7</v>
+      </c>
       <c r="Q20" s="2" t="n">
         <v>1</v>
       </c>
@@ -2280,38 +2314,38 @@
         <v>8</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="n">
         <v>6</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N21" s="3" t="s">
         <v>21</v>
@@ -2319,7 +2353,10 @@
       <c r="O21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P21" s="3"/>
+      <c r="P21" s="3" t="str">
+        <f aca="false">DEC2HEX(A21)</f>
+        <v>8</v>
+      </c>
       <c r="Q21" s="2" t="n">
         <v>0</v>
       </c>
@@ -2377,38 +2414,38 @@
         <v>9</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="n">
         <v>7</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N22" s="3" t="s">
         <v>21</v>
@@ -2416,7 +2453,10 @@
       <c r="O22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P22" s="3"/>
+      <c r="P22" s="3" t="str">
+        <f aca="false">DEC2HEX(A22)</f>
+        <v>9</v>
+      </c>
       <c r="Q22" s="2" t="n">
         <v>0</v>
       </c>
@@ -2474,16 +2514,16 @@
         <v>10</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F23" s="3" t="n">
         <v>3</v>
@@ -2492,22 +2532,22 @@
         <v>0</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N23" s="3" t="s">
         <v>21</v>
@@ -2515,7 +2555,10 @@
       <c r="O23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P23" s="3"/>
+      <c r="P23" s="3" t="str">
+        <f aca="false">DEC2HEX(A23)</f>
+        <v>A</v>
+      </c>
       <c r="Q23" s="2" t="n">
         <v>1</v>
       </c>
@@ -2573,38 +2616,38 @@
         <v>11</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>21</v>
@@ -2612,7 +2655,10 @@
       <c r="O24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P24" s="3"/>
+      <c r="P24" s="3" t="str">
+        <f aca="false">DEC2HEX(A24)</f>
+        <v>B</v>
+      </c>
       <c r="Q24" s="2" t="n">
         <v>1</v>
       </c>
@@ -2670,38 +2716,38 @@
         <v>12</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N25" s="3" t="s">
         <v>21</v>
@@ -2709,7 +2755,10 @@
       <c r="O25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P25" s="3"/>
+      <c r="P25" s="3" t="str">
+        <f aca="false">DEC2HEX(A25)</f>
+        <v>C</v>
+      </c>
       <c r="Q25" s="2" t="n">
         <v>1</v>
       </c>
@@ -2767,38 +2816,38 @@
         <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="n">
         <v>4</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N26" s="3" t="s">
         <v>21</v>
@@ -2806,7 +2855,10 @@
       <c r="O26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P26" s="3"/>
+      <c r="P26" s="3" t="str">
+        <f aca="false">DEC2HEX(A26)</f>
+        <v>D</v>
+      </c>
       <c r="Q26" s="2" t="n">
         <v>0</v>
       </c>
@@ -2864,38 +2916,38 @@
         <v>14</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="n">
         <v>5</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N27" s="3" t="s">
         <v>21</v>
@@ -2903,7 +2955,10 @@
       <c r="O27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P27" s="3"/>
+      <c r="P27" s="3" t="str">
+        <f aca="false">DEC2HEX(A27)</f>
+        <v>E</v>
+      </c>
       <c r="Q27" s="2" t="n">
         <v>0</v>
       </c>
@@ -2961,16 +3016,16 @@
         <v>15</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F28" s="3" t="n">
         <v>23</v>
@@ -2979,30 +3034,33 @@
         <v>0</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N28" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="P28" s="3"/>
+        <v>150</v>
+      </c>
+      <c r="P28" s="3" t="str">
+        <f aca="false">DEC2HEX(A28)</f>
+        <v>F</v>
+      </c>
       <c r="Q28" s="2" t="n">
         <v>1</v>
       </c>
@@ -3060,46 +3118,49 @@
         <v>16</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N29" s="3" t="s">
         <v>22</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="P29" s="3"/>
+        <v>150</v>
+      </c>
+      <c r="P29" s="3" t="str">
+        <f aca="false">DEC2HEX(A29)</f>
+        <v>10</v>
+      </c>
       <c r="Q29" s="2" t="n">
         <v>1</v>
       </c>
@@ -3157,46 +3218,49 @@
         <v>17</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N30" s="3" t="s">
         <v>22</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="P30" s="3"/>
+        <v>150</v>
+      </c>
+      <c r="P30" s="3" t="str">
+        <f aca="false">DEC2HEX(A30)</f>
+        <v>11</v>
+      </c>
       <c r="Q30" s="2" t="n">
         <v>1</v>
       </c>
@@ -3254,16 +3318,16 @@
         <v>18</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F31" s="3" t="n">
         <v>13</v>
@@ -3272,22 +3336,22 @@
         <v>0</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N31" s="3" t="s">
         <v>21</v>
@@ -3295,7 +3359,10 @@
       <c r="O31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P31" s="3"/>
+      <c r="P31" s="3" t="str">
+        <f aca="false">DEC2HEX(A31)</f>
+        <v>12</v>
+      </c>
       <c r="Q31" s="2" t="n">
         <v>1</v>
       </c>
@@ -3353,38 +3420,38 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N32" s="3" t="s">
         <v>21</v>
@@ -3392,7 +3459,10 @@
       <c r="O32" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P32" s="3"/>
+      <c r="P32" s="3" t="str">
+        <f aca="false">DEC2HEX(A32)</f>
+        <v>13</v>
+      </c>
       <c r="Q32" s="2" t="n">
         <v>1</v>
       </c>
@@ -3450,38 +3520,38 @@
         <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="n">
         <v>3</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N33" s="3" t="s">
         <v>21</v>
@@ -3489,7 +3559,10 @@
       <c r="O33" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P33" s="3"/>
+      <c r="P33" s="3" t="str">
+        <f aca="false">DEC2HEX(A33)</f>
+        <v>14</v>
+      </c>
       <c r="Q33" s="2" t="n">
         <v>0</v>
       </c>
@@ -3547,38 +3620,38 @@
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="n">
         <v>4</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N34" s="3" t="s">
         <v>21</v>
@@ -3586,7 +3659,10 @@
       <c r="O34" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P34" s="3"/>
+      <c r="P34" s="3" t="str">
+        <f aca="false">DEC2HEX(A34)</f>
+        <v>15</v>
+      </c>
       <c r="Q34" s="2" t="n">
         <v>0</v>
       </c>
@@ -3644,38 +3720,38 @@
         <v>22</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="n">
         <v>6</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N35" s="3" t="s">
         <v>21</v>
@@ -3683,7 +3759,10 @@
       <c r="O35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P35" s="3"/>
+      <c r="P35" s="3" t="str">
+        <f aca="false">DEC2HEX(A35)</f>
+        <v>16</v>
+      </c>
       <c r="Q35" s="2" t="n">
         <v>0</v>
       </c>
@@ -3741,38 +3820,38 @@
         <v>23</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="n">
         <v>7</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N36" s="3" t="s">
         <v>21</v>
@@ -3780,7 +3859,10 @@
       <c r="O36" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P36" s="3"/>
+      <c r="P36" s="3" t="str">
+        <f aca="false">DEC2HEX(A36)</f>
+        <v>17</v>
+      </c>
       <c r="Q36" s="2" t="n">
         <v>0</v>
       </c>
@@ -3838,38 +3920,38 @@
         <v>24</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I37" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N37" s="3" t="s">
         <v>21</v>
@@ -3877,7 +3959,10 @@
       <c r="O37" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P37" s="3"/>
+      <c r="P37" s="3" t="str">
+        <f aca="false">DEC2HEX(A37)</f>
+        <v>18</v>
+      </c>
       <c r="Q37" s="2" t="n">
         <v>0</v>
       </c>
@@ -3935,38 +4020,38 @@
         <v>25</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="n">
         <v>5</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I38" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N38" s="3" t="s">
         <v>21</v>
@@ -3974,7 +4059,10 @@
       <c r="O38" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P38" s="3"/>
+      <c r="P38" s="3" t="str">
+        <f aca="false">DEC2HEX(A38)</f>
+        <v>19</v>
+      </c>
       <c r="Q38" s="2" t="n">
         <v>0</v>
       </c>
@@ -4032,38 +4120,38 @@
         <v>26</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="n">
         <v>5</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I39" s="3" t="n">
         <v>1</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N39" s="3" t="s">
         <v>21</v>
@@ -4071,7 +4159,10 @@
       <c r="O39" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P39" s="3"/>
+      <c r="P39" s="3" t="str">
+        <f aca="false">DEC2HEX(A39)</f>
+        <v>1A</v>
+      </c>
       <c r="Q39" s="2" t="n">
         <v>0</v>
       </c>
@@ -4129,16 +4220,16 @@
         <v>27</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F40" s="3" t="n">
         <v>33</v>
@@ -4147,22 +4238,22 @@
         <v>0</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I40" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N40" s="3" t="s">
         <v>21</v>
@@ -4170,7 +4261,10 @@
       <c r="O40" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P40" s="3"/>
+      <c r="P40" s="3" t="str">
+        <f aca="false">DEC2HEX(A40)</f>
+        <v>1B</v>
+      </c>
       <c r="Q40" s="2" t="n">
         <v>0</v>
       </c>
@@ -4228,38 +4322,38 @@
         <v>28</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I41" s="3" t="n">
         <v>1</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N41" s="3" t="s">
         <v>21</v>
@@ -4267,7 +4361,10 @@
       <c r="O41" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P41" s="3"/>
+      <c r="P41" s="3" t="str">
+        <f aca="false">DEC2HEX(A41)</f>
+        <v>1C</v>
+      </c>
       <c r="Q41" s="2" t="n">
         <v>0</v>
       </c>
@@ -4325,38 +4422,38 @@
         <v>29</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I42" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N42" s="3" t="s">
         <v>21</v>
@@ -4364,7 +4461,10 @@
       <c r="O42" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P42" s="3"/>
+      <c r="P42" s="3" t="str">
+        <f aca="false">DEC2HEX(A42)</f>
+        <v>1D</v>
+      </c>
       <c r="Q42" s="2" t="n">
         <v>0</v>
       </c>
@@ -4422,38 +4522,38 @@
         <v>30</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I43" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N43" s="3" t="s">
         <v>21</v>
@@ -4461,7 +4561,10 @@
       <c r="O43" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P43" s="3"/>
+      <c r="P43" s="3" t="str">
+        <f aca="false">DEC2HEX(A43)</f>
+        <v>1E</v>
+      </c>
       <c r="Q43" s="2" t="n">
         <v>0</v>
       </c>
@@ -4519,38 +4622,38 @@
         <v>31</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="n">
         <v>3</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I44" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N44" s="3" t="s">
         <v>21</v>
@@ -4558,7 +4661,10 @@
       <c r="O44" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P44" s="3"/>
+      <c r="P44" s="3" t="str">
+        <f aca="false">DEC2HEX(A44)</f>
+        <v>1F</v>
+      </c>
       <c r="Q44" s="2" t="n">
         <v>1</v>
       </c>
@@ -4616,38 +4722,38 @@
         <v>32</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="n">
         <v>4</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I45" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N45" s="3" t="s">
         <v>21</v>
@@ -4655,7 +4761,10 @@
       <c r="O45" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P45" s="3"/>
+      <c r="P45" s="3" t="str">
+        <f aca="false">DEC2HEX(A45)</f>
+        <v>20</v>
+      </c>
       <c r="Q45" s="2" t="n">
         <v>0</v>
       </c>
@@ -4713,38 +4822,38 @@
         <v>33</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3" t="n">
         <v>5</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I46" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N46" s="3" t="s">
         <v>21</v>
@@ -4752,7 +4861,10 @@
       <c r="O46" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P46" s="3"/>
+      <c r="P46" s="3" t="str">
+        <f aca="false">DEC2HEX(A46)</f>
+        <v>21</v>
+      </c>
       <c r="Q46" s="2" t="n">
         <v>0</v>
       </c>
@@ -4810,38 +4922,38 @@
         <v>34</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3" t="n">
         <v>5</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I47" s="3" t="n">
         <v>1</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N47" s="3" t="s">
         <v>21</v>
@@ -4849,7 +4961,10 @@
       <c r="O47" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P47" s="3"/>
+      <c r="P47" s="3" t="str">
+        <f aca="false">DEC2HEX(A47)</f>
+        <v>22</v>
+      </c>
       <c r="Q47" s="2" t="n">
         <v>0</v>
       </c>
@@ -4907,38 +5022,38 @@
         <v>35</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3" t="n">
         <v>6</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I48" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N48" s="3" t="s">
         <v>21</v>
@@ -4946,7 +5061,10 @@
       <c r="O48" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P48" s="3"/>
+      <c r="P48" s="3" t="str">
+        <f aca="false">DEC2HEX(A48)</f>
+        <v>23</v>
+      </c>
       <c r="Q48" s="2" t="n">
         <v>0</v>
       </c>
@@ -5004,38 +5122,38 @@
         <v>36</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3" t="n">
         <v>7</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I49" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N49" s="3" t="s">
         <v>21</v>
@@ -5043,7 +5161,10 @@
       <c r="O49" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P49" s="3"/>
+      <c r="P49" s="3" t="str">
+        <f aca="false">DEC2HEX(A49)</f>
+        <v>24</v>
+      </c>
       <c r="Q49" s="2" t="n">
         <v>0</v>
       </c>
@@ -5101,46 +5222,49 @@
         <v>37</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G50" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P50" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="P50" s="3" t="str">
+        <f aca="false">DEC2HEX(A50)</f>
+        <v>25</v>
+      </c>
       <c r="Q50" s="2" t="n">
         <v>0</v>
       </c>
@@ -5198,13 +5322,13 @@
         <v>38</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -5212,30 +5336,33 @@
         <v>1</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N51" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P51" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="P51" s="3" t="str">
+        <f aca="false">DEC2HEX(A51)</f>
+        <v>26</v>
+      </c>
       <c r="Q51" s="2" t="n">
         <v>0</v>
       </c>
@@ -5293,7 +5420,7 @@
         <v>39</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -5305,30 +5432,33 @@
         <v>0</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N52" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P52" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="P52" s="3" t="str">
+        <f aca="false">DEC2HEX(A52)</f>
+        <v>27</v>
+      </c>
       <c r="Q52" s="2" t="n">
         <v>0</v>
       </c>
@@ -5382,44 +5512,47 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="n">
+      <c r="A53" s="6" t="n">
         <v>40</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I53" s="6" t="s">
+      <c r="B53" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="J53" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="K53" s="6" t="s">
+      <c r="I53" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J53" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="L53" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="M53" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="N53" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O53" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="P53" s="6"/>
+      <c r="K53" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="L53" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="M53" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="N53" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="O53" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="P53" s="7" t="str">
+        <f aca="false">DEC2HEX(A53)</f>
+        <v>28</v>
+      </c>
       <c r="Q53" s="2" t="n">
         <v>0</v>
       </c>
@@ -5465,9 +5598,9 @@
       <c r="AE53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AF53" s="6"/>
-      <c r="AG53" s="6"/>
-      <c r="AH53" s="6" t="str">
+      <c r="AF53" s="7"/>
+      <c r="AG53" s="7"/>
+      <c r="AH53" s="7" t="str">
         <f aca="false">HEX2BIN(Q53,1)&amp;HEX2BIN(R53,2)&amp;HEX2BIN(S53,2)&amp;HEX2BIN(T53,2)&amp;HEX2BIN(U53,4)&amp;HEX2BIN(V53,1)&amp;HEX2BIN(W53,1)&amp;HEX2BIN(X53,3)&amp;HEX2BIN(Y53,1)&amp;HEX2BIN(Z53,3)&amp;HEX2BIN(AA53,1)&amp;HEX2BIN(AB53,1)&amp;HEX2BIN(AC53,1)&amp;HEX2BIN(AD53,1)&amp;HEX2BIN(AE53,2)</f>
         <v>00000000000000000000000000</v>
       </c>

</xml_diff>